<commit_message>
Inserted the graphs for GCC
</commit_message>
<xml_diff>
--- a/graphs/cdc_rollingHash.xlsx
+++ b/graphs/cdc_rollingHash.xlsx
@@ -24,9 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>KR</t>
+  </si>
+  <si>
+    <t>Divisor</t>
+  </si>
+  <si>
+    <t>Block Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio </t>
   </si>
 </sst>
 </file>
@@ -381,16 +390,30 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>

</xml_diff>

<commit_message>
Updated the code for localMaxima so make it run faster
</commit_message>
<xml_diff>
--- a/graphs/cdc_rollingHash.xlsx
+++ b/graphs/cdc_rollingHash.xlsx
@@ -5,22 +5,24 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shah\Documents\thesis_git\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GCC" sheetId="1" r:id="rId1"/>
     <sheet name="emacs" sheetId="2" r:id="rId2"/>
+    <sheet name="gcc_2min" sheetId="3" r:id="rId3"/>
+    <sheet name="emacs_2min" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
   <si>
     <t>gcc</t>
   </si>
@@ -60,11 +62,17 @@
   <si>
     <t>emacs</t>
   </si>
+  <si>
+    <t>less than or equal</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,7 +122,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -153,7 +161,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -348,6 +355,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA23-4ACD-8964-CCFB2D20754D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -508,6 +520,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DA23-4ACD-8964-CCFB2D20754D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -668,6 +685,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DA23-4ACD-8964-CCFB2D20754D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -702,61 +724,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>192.452095012977</c:v>
+                  <c:v>223.19431826261399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>287.080437345039</c:v>
+                  <c:v>340.81040327152903</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>382.72724809667</c:v>
+                  <c:v>461.78751225890801</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>477.09542867757602</c:v>
+                  <c:v>584.77345641959698</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>571.48960271866702</c:v>
+                  <c:v>709.21176824982399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>675.43654967964005</c:v>
+                  <c:v>848.10758885686801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>768.84994285092296</c:v>
+                  <c:v>976.87355209017596</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>867.58874831101798</c:v>
+                  <c:v>1110.4099359352199</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>966.81130654985998</c:v>
+                  <c:v>1242.0715730238201</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1064.3119231493699</c:v>
+                  <c:v>1377.14647818669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1160.5389418337199</c:v>
+                  <c:v>1512.9142122737401</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1261.2008392482501</c:v>
+                  <c:v>1653.4300930531899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1362.14068752712</c:v>
+                  <c:v>1793.2186607426199</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1459.0043379467099</c:v>
+                  <c:v>1920.7396831871599</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1556.1641421096101</c:v>
+                  <c:v>2054.7025454545401</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1660.52427412719</c:v>
+                  <c:v>2196.3896447174002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1763.9960039959999</c:v>
+                  <c:v>2335.27525210778</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1871.3757700205299</c:v>
+                  <c:v>2481.30686808361</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1980.1065320998</c:v>
+                  <c:v>2632.51584047707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -768,66 +790,71 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.93344186780763005</c:v>
+                  <c:v>0.89836957598994205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.92299909104294997</c:v>
+                  <c:v>0.88550089621466099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91345107772290701</c:v>
+                  <c:v>0.87308428806859295</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.90384034353479503</c:v>
+                  <c:v>0.85978926920985799</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.89624046444590399</c:v>
+                  <c:v>0.84855419904177198</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.88148435376268597</c:v>
+                  <c:v>0.827863214706415</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.874060178053643</c:v>
+                  <c:v>0.81863655734641105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86429161522517195</c:v>
+                  <c:v>0.80809085039869499</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.854725090046212</c:v>
+                  <c:v>0.79844217220913305</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.84885219395614397</c:v>
+                  <c:v>0.78946066424655603</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.84183520835221104</c:v>
+                  <c:v>0.78241231820859003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.83363300363582804</c:v>
+                  <c:v>0.77467988288329104</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.82585051903995998</c:v>
+                  <c:v>0.76701717673976</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.81837664801558496</c:v>
+                  <c:v>0.75999523576250405</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.81146376064697401</c:v>
+                  <c:v>0.75356570966609204</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.80536886383200401</c:v>
+                  <c:v>0.74758439708680602</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.79695906436888397</c:v>
+                  <c:v>0.740490744778452</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.79005392861997104</c:v>
+                  <c:v>0.73207641468829199</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.78281009310438598</c:v>
+                  <c:v>0.72507829489851305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DA23-4ACD-8964-CCFB2D20754D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -888,7 +915,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1007,7 +1033,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1088,7 +1113,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1156,7 +1180,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1195,7 +1219,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1390,6 +1413,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A38F-4A54-BB59-EB5DC7304550}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1550,6 +1578,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A38F-4A54-BB59-EB5DC7304550}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1710,6 +1743,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A38F-4A54-BB59-EB5DC7304550}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1744,61 +1782,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>191.984987098288</c:v>
+                  <c:v>219.53942515323399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>287.24471352110203</c:v>
+                  <c:v>335.316446620438</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>384.43439764200201</c:v>
+                  <c:v>454.05381414701799</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>480.64600431648302</c:v>
+                  <c:v>574.96364466612795</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>578.74482904925196</c:v>
+                  <c:v>700.78732741089505</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>680.67948851231904</c:v>
+                  <c:v>829.04376012965895</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>773.01723730814604</c:v>
+                  <c:v>954.46747718592303</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>869.79329401137102</c:v>
+                  <c:v>1084.37495859556</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>970.39601612520801</c:v>
+                  <c:v>1214.20072694903</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1074.6218487394999</c:v>
+                  <c:v>1357.1544648039101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1172.83273026905</c:v>
+                  <c:v>1492.87610014136</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1273.03157567273</c:v>
+                  <c:v>1627.1013916500899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1372.74740020127</c:v>
+                  <c:v>1762.0582377953599</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1474.7186810216699</c:v>
+                  <c:v>1902.8877005347499</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1575.87753923173</c:v>
+                  <c:v>2038.1820445772601</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1681.5080384200501</c:v>
+                  <c:v>2180.74074074074</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1794.9054224464101</c:v>
+                  <c:v>2331.5490349690099</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1909.3246238189699</c:v>
+                  <c:v>2479.9090977956198</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2022.94259408021</c:v>
+                  <c:v>2621.4990390775101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1810,66 +1848,71 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.60336387140287795</c:v>
+                  <c:v>0.565048501280497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56832152823936499</c:v>
+                  <c:v>0.52979819948389095</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54131711614404099</c:v>
+                  <c:v>0.50263433614521402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51826300169103801</c:v>
+                  <c:v>0.47959082122888602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.49873040765756999</c:v>
+                  <c:v>0.458612230460197</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47784950368509499</c:v>
+                  <c:v>0.44094213080622402</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46489082171762602</c:v>
+                  <c:v>0.42703850167148799</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.45240603373279598</c:v>
+                  <c:v>0.41399859731779698</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.43866949239521402</c:v>
+                  <c:v>0.40188879467078498</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.425640370855489</c:v>
+                  <c:v>0.38752608646778203</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.41801493587738497</c:v>
+                  <c:v>0.37757128875703699</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.40868673267907402</c:v>
+                  <c:v>0.36833594605294001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.40073653034094497</c:v>
+                  <c:v>0.360014087914451</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.39371988143181103</c:v>
+                  <c:v>0.35226882013410998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.38691870552471103</c:v>
+                  <c:v>0.34549443325774098</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.38109879623475101</c:v>
+                  <c:v>0.33895338891929899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.37420353798482903</c:v>
+                  <c:v>0.33179876275609899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.36790930706521702</c:v>
+                  <c:v>0.32516143674734099</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.36179673448741001</c:v>
+                  <c:v>0.31920437495112602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A38F-4A54-BB59-EB5DC7304550}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1930,7 +1973,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2049,7 +2091,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2130,7 +2171,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3457,6 +3497,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3492,6 +3549,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3646,8 +3720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView topLeftCell="F3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,10 +3840,10 @@
         <v>100</v>
       </c>
       <c r="M5">
-        <v>192.452095012977</v>
+        <v>223.19431826261399</v>
       </c>
       <c r="N5">
-        <v>0.93344186780763005</v>
+        <v>0.89836957598994205</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3810,10 +3884,10 @@
         <v>150</v>
       </c>
       <c r="M6">
-        <v>287.080437345039</v>
+        <v>340.81040327152903</v>
       </c>
       <c r="N6">
-        <v>0.92299909104294997</v>
+        <v>0.88550089621466099</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -3854,10 +3928,10 @@
         <v>200</v>
       </c>
       <c r="M7">
-        <v>382.72724809667</v>
+        <v>461.78751225890801</v>
       </c>
       <c r="N7">
-        <v>0.91345107772290701</v>
+        <v>0.87308428806859295</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3898,10 +3972,10 @@
         <v>250</v>
       </c>
       <c r="M8">
-        <v>477.09542867757602</v>
+        <v>584.77345641959698</v>
       </c>
       <c r="N8">
-        <v>0.90384034353479503</v>
+        <v>0.85978926920985799</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -3942,10 +4016,10 @@
         <v>300</v>
       </c>
       <c r="M9">
-        <v>571.48960271866702</v>
+        <v>709.21176824982399</v>
       </c>
       <c r="N9">
-        <v>0.89624046444590399</v>
+        <v>0.84855419904177198</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -3986,10 +4060,10 @@
         <v>350</v>
       </c>
       <c r="M10">
-        <v>675.43654967964005</v>
+        <v>848.10758885686801</v>
       </c>
       <c r="N10">
-        <v>0.88148435376268597</v>
+        <v>0.827863214706415</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4030,10 +4104,10 @@
         <v>400</v>
       </c>
       <c r="M11">
-        <v>768.84994285092296</v>
+        <v>976.87355209017596</v>
       </c>
       <c r="N11">
-        <v>0.874060178053643</v>
+        <v>0.81863655734641105</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -4074,10 +4148,10 @@
         <v>450</v>
       </c>
       <c r="M12">
-        <v>867.58874831101798</v>
+        <v>1110.4099359352199</v>
       </c>
       <c r="N12">
-        <v>0.86429161522517195</v>
+        <v>0.80809085039869499</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -4118,10 +4192,10 @@
         <v>500</v>
       </c>
       <c r="M13">
-        <v>966.81130654985998</v>
+        <v>1242.0715730238201</v>
       </c>
       <c r="N13">
-        <v>0.854725090046212</v>
+        <v>0.79844217220913305</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4162,10 +4236,10 @@
         <v>550</v>
       </c>
       <c r="M14">
-        <v>1064.3119231493699</v>
+        <v>1377.14647818669</v>
       </c>
       <c r="N14">
-        <v>0.84885219395614397</v>
+        <v>0.78946066424655603</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4206,10 +4280,10 @@
         <v>600</v>
       </c>
       <c r="M15">
-        <v>1160.5389418337199</v>
+        <v>1512.9142122737401</v>
       </c>
       <c r="N15">
-        <v>0.84183520835221104</v>
+        <v>0.78241231820859003</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -4250,10 +4324,10 @@
         <v>650</v>
       </c>
       <c r="M16">
-        <v>1261.2008392482501</v>
+        <v>1653.4300930531899</v>
       </c>
       <c r="N16">
-        <v>0.83363300363582804</v>
+        <v>0.77467988288329104</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -4294,10 +4368,10 @@
         <v>700</v>
       </c>
       <c r="M17">
-        <v>1362.14068752712</v>
+        <v>1793.2186607426199</v>
       </c>
       <c r="N17">
-        <v>0.82585051903995998</v>
+        <v>0.76701717673976</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -4338,10 +4412,10 @@
         <v>750</v>
       </c>
       <c r="M18">
-        <v>1459.0043379467099</v>
+        <v>1920.7396831871599</v>
       </c>
       <c r="N18">
-        <v>0.81837664801558496</v>
+        <v>0.75999523576250405</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -4382,10 +4456,10 @@
         <v>800</v>
       </c>
       <c r="M19">
-        <v>1556.1641421096101</v>
+        <v>2054.7025454545401</v>
       </c>
       <c r="N19">
-        <v>0.81146376064697401</v>
+        <v>0.75356570966609204</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4426,10 +4500,10 @@
         <v>850</v>
       </c>
       <c r="M20">
-        <v>1660.52427412719</v>
+        <v>2196.3896447174002</v>
       </c>
       <c r="N20">
-        <v>0.80536886383200401</v>
+        <v>0.74758439708680602</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -4470,10 +4544,10 @@
         <v>900</v>
       </c>
       <c r="M21">
-        <v>1763.9960039959999</v>
+        <v>2335.27525210778</v>
       </c>
       <c r="N21">
-        <v>0.79695906436888397</v>
+        <v>0.740490744778452</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -4514,10 +4588,10 @@
         <v>950</v>
       </c>
       <c r="M22">
-        <v>1871.3757700205299</v>
+        <v>2481.30686808361</v>
       </c>
       <c r="N22">
-        <v>0.79005392861997104</v>
+        <v>0.73207641468829199</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -4558,10 +4632,10 @@
         <v>1000</v>
       </c>
       <c r="M23">
-        <v>1980.1065320998</v>
+        <v>2632.51584047707</v>
       </c>
       <c r="N23">
-        <v>0.78281009310438598</v>
+        <v>0.72507829489851305</v>
       </c>
     </row>
   </sheetData>
@@ -4575,8 +4649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4695,10 +4769,10 @@
         <v>100</v>
       </c>
       <c r="M5">
-        <v>191.984987098288</v>
+        <v>219.53942515323399</v>
       </c>
       <c r="N5">
-        <v>0.60336387140287795</v>
+        <v>0.565048501280497</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4739,10 +4813,10 @@
         <v>150</v>
       </c>
       <c r="M6">
-        <v>287.24471352110203</v>
+        <v>335.316446620438</v>
       </c>
       <c r="N6">
-        <v>0.56832152823936499</v>
+        <v>0.52979819948389095</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4783,10 +4857,10 @@
         <v>200</v>
       </c>
       <c r="M7">
-        <v>384.43439764200201</v>
+        <v>454.05381414701799</v>
       </c>
       <c r="N7">
-        <v>0.54131711614404099</v>
+        <v>0.50263433614521402</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4827,10 +4901,10 @@
         <v>250</v>
       </c>
       <c r="M8">
-        <v>480.64600431648302</v>
+        <v>574.96364466612795</v>
       </c>
       <c r="N8">
-        <v>0.51826300169103801</v>
+        <v>0.47959082122888602</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4871,10 +4945,10 @@
         <v>300</v>
       </c>
       <c r="M9">
-        <v>578.74482904925196</v>
+        <v>700.78732741089505</v>
       </c>
       <c r="N9">
-        <v>0.49873040765756999</v>
+        <v>0.458612230460197</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4915,10 +4989,10 @@
         <v>350</v>
       </c>
       <c r="M10">
-        <v>680.67948851231904</v>
+        <v>829.04376012965895</v>
       </c>
       <c r="N10">
-        <v>0.47784950368509499</v>
+        <v>0.44094213080622402</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4959,10 +5033,10 @@
         <v>400</v>
       </c>
       <c r="M11">
-        <v>773.01723730814604</v>
+        <v>954.46747718592303</v>
       </c>
       <c r="N11">
-        <v>0.46489082171762602</v>
+        <v>0.42703850167148799</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -5003,10 +5077,10 @@
         <v>450</v>
       </c>
       <c r="M12">
-        <v>869.79329401137102</v>
+        <v>1084.37495859556</v>
       </c>
       <c r="N12">
-        <v>0.45240603373279598</v>
+        <v>0.41399859731779698</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -5047,10 +5121,10 @@
         <v>500</v>
       </c>
       <c r="M13">
-        <v>970.39601612520801</v>
+        <v>1214.20072694903</v>
       </c>
       <c r="N13">
-        <v>0.43866949239521402</v>
+        <v>0.40188879467078498</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -5091,10 +5165,10 @@
         <v>550</v>
       </c>
       <c r="M14">
-        <v>1074.6218487394999</v>
+        <v>1357.1544648039101</v>
       </c>
       <c r="N14">
-        <v>0.425640370855489</v>
+        <v>0.38752608646778203</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -5135,10 +5209,10 @@
         <v>600</v>
       </c>
       <c r="M15">
-        <v>1172.83273026905</v>
+        <v>1492.87610014136</v>
       </c>
       <c r="N15">
-        <v>0.41801493587738497</v>
+        <v>0.37757128875703699</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -5179,10 +5253,10 @@
         <v>650</v>
       </c>
       <c r="M16">
-        <v>1273.03157567273</v>
+        <v>1627.1013916500899</v>
       </c>
       <c r="N16">
-        <v>0.40868673267907402</v>
+        <v>0.36833594605294001</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -5223,10 +5297,10 @@
         <v>700</v>
       </c>
       <c r="M17">
-        <v>1372.74740020127</v>
+        <v>1762.0582377953599</v>
       </c>
       <c r="N17">
-        <v>0.40073653034094497</v>
+        <v>0.360014087914451</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -5267,10 +5341,10 @@
         <v>750</v>
       </c>
       <c r="M18">
-        <v>1474.7186810216699</v>
+        <v>1902.8877005347499</v>
       </c>
       <c r="N18">
-        <v>0.39371988143181103</v>
+        <v>0.35226882013410998</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -5311,10 +5385,10 @@
         <v>800</v>
       </c>
       <c r="M19">
-        <v>1575.87753923173</v>
+        <v>2038.1820445772601</v>
       </c>
       <c r="N19">
-        <v>0.38691870552471103</v>
+        <v>0.34549443325774098</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -5355,10 +5429,10 @@
         <v>850</v>
       </c>
       <c r="M20">
-        <v>1681.5080384200501</v>
+        <v>2180.74074074074</v>
       </c>
       <c r="N20">
-        <v>0.38109879623475101</v>
+        <v>0.33895338891929899</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -5399,10 +5473,10 @@
         <v>900</v>
       </c>
       <c r="M21">
-        <v>1794.9054224464101</v>
+        <v>2331.5490349690099</v>
       </c>
       <c r="N21">
-        <v>0.37420353798482903</v>
+        <v>0.33179876275609899</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -5443,10 +5517,10 @@
         <v>950</v>
       </c>
       <c r="M22">
-        <v>1909.3246238189699</v>
+        <v>2479.9090977956198</v>
       </c>
       <c r="N22">
-        <v>0.36790930706521702</v>
+        <v>0.32516143674734099</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -5487,10 +5561,10 @@
         <v>1000</v>
       </c>
       <c r="M23">
-        <v>2022.94259408021</v>
+        <v>2621.4990390775101</v>
       </c>
       <c r="N23">
-        <v>0.36179673448741001</v>
+        <v>0.31920437495112602</v>
       </c>
     </row>
   </sheetData>
@@ -5502,4 +5576,875 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>192.452095012977</v>
+      </c>
+      <c r="C7">
+        <v>0.93344186780763005</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>223.19431826261399</v>
+      </c>
+      <c r="F7">
+        <v>0.89836957598994205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>150</v>
+      </c>
+      <c r="B8">
+        <v>287.080437345039</v>
+      </c>
+      <c r="C8">
+        <v>0.92299909104294997</v>
+      </c>
+      <c r="D8">
+        <v>150</v>
+      </c>
+      <c r="E8">
+        <v>340.81040327152903</v>
+      </c>
+      <c r="F8">
+        <v>0.88550089621466099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>200</v>
+      </c>
+      <c r="B9">
+        <v>382.72724809667</v>
+      </c>
+      <c r="C9">
+        <v>0.91345107772290701</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <v>461.78751225890801</v>
+      </c>
+      <c r="F9">
+        <v>0.87308428806859295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>250</v>
+      </c>
+      <c r="B10">
+        <v>477.09542867757602</v>
+      </c>
+      <c r="C10">
+        <v>0.90384034353479503</v>
+      </c>
+      <c r="D10">
+        <v>250</v>
+      </c>
+      <c r="E10">
+        <v>584.77345641959698</v>
+      </c>
+      <c r="F10">
+        <v>0.85978926920985799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11">
+        <v>571.48960271866702</v>
+      </c>
+      <c r="C11">
+        <v>0.89624046444590399</v>
+      </c>
+      <c r="D11">
+        <v>300</v>
+      </c>
+      <c r="E11">
+        <v>709.21176824982399</v>
+      </c>
+      <c r="F11">
+        <v>0.84855419904177198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>350</v>
+      </c>
+      <c r="B12">
+        <v>675.43654967964005</v>
+      </c>
+      <c r="C12">
+        <v>0.88148435376268597</v>
+      </c>
+      <c r="D12">
+        <v>350</v>
+      </c>
+      <c r="E12">
+        <v>848.10758885686801</v>
+      </c>
+      <c r="F12">
+        <v>0.827863214706415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>400</v>
+      </c>
+      <c r="B13">
+        <v>768.84994285092296</v>
+      </c>
+      <c r="C13">
+        <v>0.874060178053643</v>
+      </c>
+      <c r="D13">
+        <v>400</v>
+      </c>
+      <c r="E13">
+        <v>976.87355209017596</v>
+      </c>
+      <c r="F13">
+        <v>0.81863655734641105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>450</v>
+      </c>
+      <c r="B14">
+        <v>867.58874831101798</v>
+      </c>
+      <c r="C14">
+        <v>0.86429161522517195</v>
+      </c>
+      <c r="D14">
+        <v>450</v>
+      </c>
+      <c r="E14">
+        <v>1110.4099359352199</v>
+      </c>
+      <c r="F14">
+        <v>0.80809085039869499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>500</v>
+      </c>
+      <c r="B15">
+        <v>966.81130654985998</v>
+      </c>
+      <c r="C15">
+        <v>0.854725090046212</v>
+      </c>
+      <c r="D15">
+        <v>500</v>
+      </c>
+      <c r="E15">
+        <v>1242.0715730238201</v>
+      </c>
+      <c r="F15">
+        <v>0.79844217220913305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>550</v>
+      </c>
+      <c r="B16">
+        <v>1064.3119231493699</v>
+      </c>
+      <c r="C16">
+        <v>0.84885219395614397</v>
+      </c>
+      <c r="D16">
+        <v>550</v>
+      </c>
+      <c r="E16">
+        <v>1377.14647818669</v>
+      </c>
+      <c r="F16">
+        <v>0.78946066424655603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>600</v>
+      </c>
+      <c r="B17">
+        <v>1160.5389418337199</v>
+      </c>
+      <c r="C17">
+        <v>0.84183520835221104</v>
+      </c>
+      <c r="D17">
+        <v>600</v>
+      </c>
+      <c r="E17">
+        <v>1512.9142122737401</v>
+      </c>
+      <c r="F17">
+        <v>0.78241231820859003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>650</v>
+      </c>
+      <c r="B18">
+        <v>1261.2008392482501</v>
+      </c>
+      <c r="C18">
+        <v>0.83363300363582804</v>
+      </c>
+      <c r="D18">
+        <v>650</v>
+      </c>
+      <c r="E18">
+        <v>1653.4300930531899</v>
+      </c>
+      <c r="F18">
+        <v>0.77467988288329104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>700</v>
+      </c>
+      <c r="B19">
+        <v>1362.14068752712</v>
+      </c>
+      <c r="C19">
+        <v>0.82585051903995998</v>
+      </c>
+      <c r="D19">
+        <v>700</v>
+      </c>
+      <c r="E19">
+        <v>1793.2186607426199</v>
+      </c>
+      <c r="F19">
+        <v>0.76701717673976</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>750</v>
+      </c>
+      <c r="B20">
+        <v>1459.0043379467099</v>
+      </c>
+      <c r="C20">
+        <v>0.81837664801558496</v>
+      </c>
+      <c r="D20">
+        <v>750</v>
+      </c>
+      <c r="E20">
+        <v>1920.7396831871599</v>
+      </c>
+      <c r="F20">
+        <v>0.75999523576250405</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>800</v>
+      </c>
+      <c r="B21">
+        <v>1556.1641421096101</v>
+      </c>
+      <c r="C21">
+        <v>0.81146376064697401</v>
+      </c>
+      <c r="D21">
+        <v>800</v>
+      </c>
+      <c r="E21">
+        <v>2054.7025454545401</v>
+      </c>
+      <c r="F21">
+        <v>0.75356570966609204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>850</v>
+      </c>
+      <c r="B22">
+        <v>1660.52427412719</v>
+      </c>
+      <c r="C22">
+        <v>0.80536886383200401</v>
+      </c>
+      <c r="D22">
+        <v>850</v>
+      </c>
+      <c r="E22">
+        <v>2196.3896447174002</v>
+      </c>
+      <c r="F22">
+        <v>0.74758439708680602</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>900</v>
+      </c>
+      <c r="B23">
+        <v>1763.9960039959999</v>
+      </c>
+      <c r="C23">
+        <v>0.79695906436888397</v>
+      </c>
+      <c r="D23">
+        <v>900</v>
+      </c>
+      <c r="E23">
+        <v>2335.27525210778</v>
+      </c>
+      <c r="F23">
+        <v>0.740490744778452</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>950</v>
+      </c>
+      <c r="B24">
+        <v>1871.3757700205299</v>
+      </c>
+      <c r="C24">
+        <v>0.79005392861997104</v>
+      </c>
+      <c r="D24">
+        <v>950</v>
+      </c>
+      <c r="E24">
+        <v>2481.30686808361</v>
+      </c>
+      <c r="F24">
+        <v>0.73207641468829199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1000</v>
+      </c>
+      <c r="B25">
+        <v>1980.1065320998</v>
+      </c>
+      <c r="C25">
+        <v>0.78281009310438598</v>
+      </c>
+      <c r="D25">
+        <v>1000</v>
+      </c>
+      <c r="E25">
+        <v>2632.51584047707</v>
+      </c>
+      <c r="F25">
+        <v>0.72507829489851305</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>191.984987098288</v>
+      </c>
+      <c r="C5">
+        <v>0.60336387140287795</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>219.53942515323399</v>
+      </c>
+      <c r="F5">
+        <v>0.565048501280497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6">
+        <v>287.24471352110203</v>
+      </c>
+      <c r="C6">
+        <v>0.56832152823936499</v>
+      </c>
+      <c r="D6">
+        <v>150</v>
+      </c>
+      <c r="E6">
+        <v>335.316446620438</v>
+      </c>
+      <c r="F6">
+        <v>0.52979819948389095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>200</v>
+      </c>
+      <c r="B7">
+        <v>384.43439764200201</v>
+      </c>
+      <c r="C7">
+        <v>0.54131711614404099</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7">
+        <v>454.05381414701799</v>
+      </c>
+      <c r="F7">
+        <v>0.50263433614521402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>480.64600431648302</v>
+      </c>
+      <c r="C8">
+        <v>0.51826300169103801</v>
+      </c>
+      <c r="D8">
+        <v>250</v>
+      </c>
+      <c r="E8">
+        <v>574.96364466612795</v>
+      </c>
+      <c r="F8">
+        <v>0.47959082122888602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>300</v>
+      </c>
+      <c r="B9">
+        <v>578.74482904925196</v>
+      </c>
+      <c r="C9">
+        <v>0.49873040765756999</v>
+      </c>
+      <c r="D9">
+        <v>300</v>
+      </c>
+      <c r="E9">
+        <v>700.78732741089505</v>
+      </c>
+      <c r="F9">
+        <v>0.458612230460197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>350</v>
+      </c>
+      <c r="B10">
+        <v>680.67948851231904</v>
+      </c>
+      <c r="C10">
+        <v>0.47784950368509499</v>
+      </c>
+      <c r="D10">
+        <v>350</v>
+      </c>
+      <c r="E10">
+        <v>829.04376012965895</v>
+      </c>
+      <c r="F10">
+        <v>0.44094213080622402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>400</v>
+      </c>
+      <c r="B11">
+        <v>773.01723730814604</v>
+      </c>
+      <c r="C11">
+        <v>0.46489082171762602</v>
+      </c>
+      <c r="D11">
+        <v>400</v>
+      </c>
+      <c r="E11">
+        <v>954.46747718592303</v>
+      </c>
+      <c r="F11">
+        <v>0.42703850167148799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>450</v>
+      </c>
+      <c r="B12">
+        <v>869.79329401137102</v>
+      </c>
+      <c r="C12">
+        <v>0.45240603373279598</v>
+      </c>
+      <c r="D12">
+        <v>450</v>
+      </c>
+      <c r="E12">
+        <v>1084.37495859556</v>
+      </c>
+      <c r="F12">
+        <v>0.41399859731779698</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>500</v>
+      </c>
+      <c r="B13">
+        <v>970.39601612520801</v>
+      </c>
+      <c r="C13">
+        <v>0.43866949239521402</v>
+      </c>
+      <c r="D13">
+        <v>500</v>
+      </c>
+      <c r="E13">
+        <v>1214.20072694903</v>
+      </c>
+      <c r="F13">
+        <v>0.40188879467078498</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>550</v>
+      </c>
+      <c r="B14">
+        <v>1074.6218487394999</v>
+      </c>
+      <c r="C14">
+        <v>0.425640370855489</v>
+      </c>
+      <c r="D14">
+        <v>550</v>
+      </c>
+      <c r="E14">
+        <v>1357.1544648039101</v>
+      </c>
+      <c r="F14">
+        <v>0.38752608646778203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>600</v>
+      </c>
+      <c r="B15">
+        <v>1172.83273026905</v>
+      </c>
+      <c r="C15">
+        <v>0.41801493587738497</v>
+      </c>
+      <c r="D15">
+        <v>600</v>
+      </c>
+      <c r="E15">
+        <v>1492.87610014136</v>
+      </c>
+      <c r="F15">
+        <v>0.37757128875703699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>650</v>
+      </c>
+      <c r="B16">
+        <v>1273.03157567273</v>
+      </c>
+      <c r="C16">
+        <v>0.40868673267907402</v>
+      </c>
+      <c r="D16">
+        <v>650</v>
+      </c>
+      <c r="E16">
+        <v>1627.1013916500899</v>
+      </c>
+      <c r="F16">
+        <v>0.36833594605294001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>700</v>
+      </c>
+      <c r="B17">
+        <v>1372.74740020127</v>
+      </c>
+      <c r="C17">
+        <v>0.40073653034094497</v>
+      </c>
+      <c r="D17">
+        <v>700</v>
+      </c>
+      <c r="E17">
+        <v>1762.0582377953599</v>
+      </c>
+      <c r="F17">
+        <v>0.360014087914451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>750</v>
+      </c>
+      <c r="B18">
+        <v>1474.7186810216699</v>
+      </c>
+      <c r="C18">
+        <v>0.39371988143181103</v>
+      </c>
+      <c r="D18">
+        <v>750</v>
+      </c>
+      <c r="E18">
+        <v>1902.8877005347499</v>
+      </c>
+      <c r="F18">
+        <v>0.35226882013410998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>800</v>
+      </c>
+      <c r="B19">
+        <v>1575.87753923173</v>
+      </c>
+      <c r="C19">
+        <v>0.38691870552471103</v>
+      </c>
+      <c r="D19">
+        <v>800</v>
+      </c>
+      <c r="E19">
+        <v>2038.1820445772601</v>
+      </c>
+      <c r="F19">
+        <v>0.34549443325774098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>850</v>
+      </c>
+      <c r="B20">
+        <v>1681.5080384200501</v>
+      </c>
+      <c r="C20">
+        <v>0.38109879623475101</v>
+      </c>
+      <c r="D20">
+        <v>850</v>
+      </c>
+      <c r="E20">
+        <v>2180.74074074074</v>
+      </c>
+      <c r="F20">
+        <v>0.33895338891929899</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>900</v>
+      </c>
+      <c r="B21">
+        <v>1794.9054224464101</v>
+      </c>
+      <c r="C21">
+        <v>0.37420353798482903</v>
+      </c>
+      <c r="D21">
+        <v>900</v>
+      </c>
+      <c r="E21">
+        <v>2331.5490349690099</v>
+      </c>
+      <c r="F21">
+        <v>0.33179876275609899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>950</v>
+      </c>
+      <c r="B22">
+        <v>1909.3246238189699</v>
+      </c>
+      <c r="C22">
+        <v>0.36790930706521702</v>
+      </c>
+      <c r="D22">
+        <v>950</v>
+      </c>
+      <c r="E22">
+        <v>2479.9090977956198</v>
+      </c>
+      <c r="F22">
+        <v>0.32516143674734099</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1000</v>
+      </c>
+      <c r="B23">
+        <v>2022.94259408021</v>
+      </c>
+      <c r="C23">
+        <v>0.36179673448741001</v>
+      </c>
+      <c r="D23">
+        <v>1000</v>
+      </c>
+      <c r="E23">
+        <v>2621.4990390775101</v>
+      </c>
+      <c r="F23">
+        <v>0.31920437495112602</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>